<commit_message>
Foot print for inductor added
</commit_message>
<xml_diff>
--- a/ESP-Counter-KiCAD_BOM_for_costing_Rev-01.xlsx
+++ b/ESP-Counter-KiCAD_BOM_for_costing_Rev-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Controller Project\ESP-Counter-KiCAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F80EECE-57DC-4BB7-9BCC-B7EE045D4249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3B470F-7DDA-4B6A-BC0B-0702004672F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3562,7 +3562,7 @@
   <dimension ref="A2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
220uF Cap added at 5V
</commit_message>
<xml_diff>
--- a/ESP-Counter-KiCAD_BOM_for_costing_Rev-01.xlsx
+++ b/ESP-Counter-KiCAD_BOM_for_costing_Rev-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Controller Project\ESP-Counter-KiCAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3B470F-7DDA-4B6A-BC0B-0702004672F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FFE9C9-8B96-41D8-B901-284233DD4BC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3562,7 +3562,7 @@
   <dimension ref="A2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>